<commit_message>
uploaded requirements.txt and README.txt
</commit_message>
<xml_diff>
--- a/DAA-work/destinations.xlsx
+++ b/DAA-work/destinations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,10 +480,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -498,6 +496,27 @@
       </c>
       <c r="E3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2356</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Destination1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12.8293764059038</v>
+      </c>
+      <c r="D4" t="n">
+        <v>80.12243270874025</v>
+      </c>
+      <c r="E4" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>